<commit_message>
Changes to the dataset (juice/nectar) & Fruit lists in R Code^
</commit_message>
<xml_diff>
--- a/JuiceDataset.xlsx
+++ b/JuiceDataset.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rene/Documents/Inferential-Statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josefine Kuka\Documents\Inferential Projekt\Inferential-Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -307,6 +307,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -577,13 +580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N3" zoomScale="91" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32:AJ32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="91" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -839,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -967,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1991,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2119,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2247,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -2375,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2887,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3143,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3527,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3783,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4039,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4167,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -4295,7 +4301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4807,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -5191,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
adjustments in the dataset
</commit_message>
<xml_diff>
--- a/JuiceDataset.xlsx
+++ b/JuiceDataset.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rene/Documents/Inferential-Statistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josefine Kuka\Documents\Inferential Projekt\Inferential-Statistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -307,6 +307,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -577,13 +580,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N3" zoomScale="91" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32:AJ32"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="91" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="27.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -711,7 +717,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -839,7 +845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -967,7 +973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1095,7 +1101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1223,7 +1229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1351,7 +1357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1479,7 +1485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1607,7 +1613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1735,7 +1741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1991,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2008,7 +2014,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -2119,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -2247,7 +2253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2264,7 +2270,7 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -2375,7 +2381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2503,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2887,7 +2893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3143,7 +3149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3271,7 +3277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3399,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3527,7 +3533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3655,7 +3661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3783,7 +3789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3911,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4039,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4167,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4184,7 +4190,7 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -4295,7 +4301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4423,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4551,7 +4557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4679,7 +4685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4807,7 +4813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4935,7 +4941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -5063,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>36</v>
       </c>
@@ -5191,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
adjusted prices of juices
</commit_message>
<xml_diff>
--- a/JuiceDataset.xlsx
+++ b/JuiceDataset.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27809"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josefine Kuka\Documents\Inferential Projekt\Inferential-Statistics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rene/Documents/Inferential-Statistics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="16005" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -266,7 +266,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -580,13 +580,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="91" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="91" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.625" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" x14ac:dyDescent="0.25">
@@ -2645,7 +2645,7 @@
         <v>57</v>
       </c>
       <c r="C17">
-        <v>7.16</v>
+        <v>5.32</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -3157,7 +3157,7 @@
         <v>61</v>
       </c>
       <c r="C21">
-        <v>7.16</v>
+        <v>5.32</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -4181,7 +4181,7 @@
         <v>69</v>
       </c>
       <c r="C29">
-        <v>7.16</v>
+        <v>5.32</v>
       </c>
       <c r="D29">
         <v>1</v>

</xml_diff>